<commit_message>
Added PDF displayer class
</commit_message>
<xml_diff>
--- a/Data/Excel/MOCK_DATA.xlsx
+++ b/Data/Excel/MOCK_DATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Documents\GitHub\2-Semester-Examproject\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3BD0AA-35B1-4693-908F-53AAB6CDE242}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26942580-2CED-4724-8462-30B38FCEF949}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28455" yWindow="5400" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="5400" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -505,7 +505,7 @@
     <t>10/31/2020</t>
   </si>
   <si>
-    <t>570-428-4322</t>
+    <t>570-428-4344</t>
   </si>
 </sst>
 </file>
@@ -858,7 +858,7 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>